<commit_message>
adds final results to final output and organizes the two notebooks
</commit_message>
<xml_diff>
--- a/output/results_cv.xlsx
+++ b/output/results_cv.xlsx
@@ -10,13 +10,14 @@
     <sheet name="Random Forest" sheetId="1" r:id="rId1"/>
     <sheet name="Ridge" sheetId="2" r:id="rId2"/>
     <sheet name="Huber" sheetId="3" r:id="rId3"/>
+    <sheet name="Final Models Results" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="124">
   <si>
     <t>MSE</t>
   </si>
@@ -364,6 +365,30 @@
   </si>
   <si>
     <t>{'alpha': 100, 'epsilon': 3}</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>Ridge</t>
+  </si>
+  <si>
+    <t>Huber</t>
+  </si>
+  <si>
+    <t>N_Estimators = 50</t>
+  </si>
+  <si>
+    <t>Alpha = 5</t>
+  </si>
+  <si>
+    <t>Alpha = 10, Epsilon = 3</t>
   </si>
 </sst>
 </file>
@@ -6000,4 +6025,70 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2">
+        <v>0.1718197289417877</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3">
+        <v>0.1956336659664253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4">
+        <v>0.2023400465004621</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>